<commit_message>
indicadores 5.4, 5.5 y 5.16
</commit_message>
<xml_diff>
--- a/Codigo/Bases/datos_administrativos/Indicadores_de_Género/VIOLENCIA/Violencia Intrafamiliar/Violencia Intrafamiliar.xlsx
+++ b/Codigo/Bases/datos_administrativos/Indicadores_de_Género/VIOLENCIA/Violencia Intrafamiliar/Violencia Intrafamiliar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ineedso\Desktop\DESA 2023\SOLICITUDES DE INFORMACION 2023\Solicitud de Genero\VIOLENCIA\Violencia Intrafamiliar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inegobgt-my.sharepoint.com/personal/unidadgenero_ine_gob_gt/Documents/Documentos/Github/CompendioGenero2023/Codigo/Bases/datos_administrativos/Indicadores_de_Género/VIOLENCIA/Violencia Intrafamiliar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93DC87A5-284F-45FF-A54A-E765BE5F35C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{93DC87A5-284F-45FF-A54A-E765BE5F35C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35C66D63-463B-4BC5-A265-0955F77D3232}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7077F3C3-D065-4AF6-B506-2EB171830680}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{7077F3C3-D065-4AF6-B506-2EB171830680}"/>
   </bookViews>
   <sheets>
     <sheet name="5.5" sheetId="3" r:id="rId1"/>
@@ -331,7 +331,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +347,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,7 +478,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -532,6 +538,22 @@
     <xf numFmtId="41" fontId="5" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,6 +605,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -884,7 +910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80AE4B9-DEE0-42A3-A087-C7AD70B29FD2}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9:P15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -913,100 +941,100 @@
       <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="33">
         <v>2018</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="27">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="33">
         <v>2019</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="27">
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="33">
         <v>2020</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="27">
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="33">
         <v>2021</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="27">
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="33">
         <v>2022</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="13" t="s">
         <v>2</v>
       </c>
@@ -1153,153 +1181,153 @@
         <v>19133</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="24">
         <v>8787</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="25">
         <v>1137</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="25">
         <v>7650</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="26">
         <v>9730</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="27">
         <v>1382</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="27">
         <v>8348</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="26">
         <v>9020</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="27">
         <v>1243</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="27">
         <v>7777</v>
       </c>
-      <c r="K10" s="21">
+      <c r="K10" s="26">
         <v>9955</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="27">
         <v>1458</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="27">
         <v>8497</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="26">
         <v>10126</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="27">
         <v>1517</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="27">
         <v>8609</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="24">
         <v>57</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="25">
         <v>11</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="25">
         <v>46</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="26">
         <v>49</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="27">
         <v>9</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="27">
         <v>40</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="26">
         <v>28</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="27">
         <v>5</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="27">
         <v>23</v>
       </c>
-      <c r="K11" s="21">
+      <c r="K11" s="26">
         <v>46</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="27">
         <v>7</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="27">
         <v>39</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="26">
         <v>46</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="27">
         <v>6</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="27">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="24">
         <v>49</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="25">
         <v>12</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="25">
         <v>37</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="26">
         <v>72</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="27">
         <v>10</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="27">
         <v>62</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="26">
         <v>18</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="27">
         <v>5</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="27">
         <v>13</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="26">
         <v>38</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="27">
         <v>2</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="27">
         <v>36</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="26">
         <v>49</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="27">
         <v>14</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="27">
         <v>35</v>
       </c>
     </row>
@@ -1483,7 +1511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08871730-6D48-4902-9894-3E1E61D760DD}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="K6" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9:O23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1512,100 +1542,100 @@
       <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="33">
         <v>2018</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="27">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="33">
         <v>2019</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="27">
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="33">
         <v>2020</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="27">
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="33">
         <v>2021</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="27">
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="33">
         <v>2022</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="13" t="s">
         <v>2</v>
       </c>
@@ -2482,7 +2512,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2C3E58-DFA4-4777-B147-061AF61DED5B}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2511,100 +2543,100 @@
       <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
       <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
       <c r="Q3" s="12"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
       <c r="Q4" s="12"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="33">
         <v>2018</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="27">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="33">
         <v>2019</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="27">
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="33">
         <v>2020</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="27">
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="33">
         <v>2021</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="27">
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="33">
         <v>2022</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3012,12 +3044,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>